<commit_message>
Phase 3.1.1 - Word-Level Diff Enhancement
CHANGES:
- Word-level diff algorithm (cleaner than character-level)
- Separate 4-column layout: Previous | Current | Analysis | Diff Detail
- Progress tracking with filling bar during analysis
- StrOrigin Analysis now in BOTH Raw and Working Process
- Optimized column widths for better readability
- All version files updated to v1.121.0
- Excel guides updated with Phase 3.1.1 features
- Test suite expanded and moved to tests/ folder
- Root directory cleaned up

TECHNICAL:
- src/utils/strorigin_analysis.py: Word-level diff + tuple returns
- src/processors/raw_processor.py: Added StrOrigin Analysis sheet
- src/processors/working_processor.py: New column layout + progress
- roadmap.md: Phase 3.1.1 complete documentation
- All tests passing (100% accuracy maintained)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_EN.xlsx
+++ b/docs/VRS_Manager_Process_Guide_EN.xlsx
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C241"/>
+  <dimension ref="A1:C276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,9 +616,9 @@
       <c r="C1" s="2" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" s="28" t="inlineStr">
-        <is>
-          <t>Version 1120.0 (Phase 3.0 - Professional Installer System)</t>
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Version 1121.0 (Phase 3.1.1 - Word-Level Diff Enhancement)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -2132,6 +2132,233 @@
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
+        </is>
+      </c>
+    </row>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244">
+      <c r="A244" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v1.121.0?</t>
+        </is>
+      </c>
+    </row>
+    <row r="245"/>
+    <row r="246">
+      <c r="A246" s="9" t="inlineStr">
+        <is>
+          <t>✅ Phase 3.1.1 COMPLETED - Word-Level Diff Enhancement (v1.121.0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IMPROVED: Word-level diff (cleaner output than character-level)</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: Separate 'Diff Detail' column showing exact changes [old→new]</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: Progress bar with filling animation during analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: StrOrigin Analysis now in BOTH Raw and Working Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IMPROVED: 4-column layout for better readability</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • ANALYSIS: Shows which StrOrigin changes are trivial vs substantial</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="9" t="inlineStr">
+        <is>
+          <t>✅ Critical Bug Fixes (v1118.6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: TypeError 'unhashable type: dict' in Working VRS Check</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: All DataFrame column access now uses safe_str() pattern</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: Lookup dictionaries now correctly store indices (not dict objects)</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: 100% accuracy verified with 5000-row comprehensive test suite</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: All processors (Raw, Working, All Language) passing with real data</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="9" t="inlineStr">
+        <is>
+          <t>✅ Phase 2.2.1 COMPLETED - Super Group Analysis Improvements (v1118.4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REMOVED: 'Others' super group and stageclosedialog check entirely</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REORDERED: Super groups - AI Dialog now appears before Quest Dialog</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • RENAMED: 'Untranslated Words (Remaining to Translate)' → 'Not Translated'</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REMOVED: Migration columns from main table (Words Migrated In/Out)</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • ADDED: Detailed 'Super Group Migrations' table below main table</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows source → destination pairs with word counts for all migrations</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • UPDATED: Explanatory notes below table (removed 'Others' references)</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 8 super groups total: Main Chapters, F1, F2, F3, AI Dialog, Quest Dialog, Other, Everything Else</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="9" t="inlineStr">
+        <is>
+          <t>Column Order (Reorganized for Better Readability):</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 1. Super Group Name, Total Words (Current/Previous), Net Change, % Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 2. Translated/Untranslated words, Translation % (Current/Previous/Change)</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 3. Detailed breakdown: Words Added/Deleted/Changed/Unchanged/Migrated</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame Preservation Restored</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame ONLY (EndFrame always updates from SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed AND StrOrigin changed → Update StartFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed BUT StrOrigin NOT changed → Preserve StartFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
         </is>
@@ -2302,6 +2529,7 @@
         </is>
       </c>
     </row>
+    <row r="20"/>
     <row r="21">
       <c r="A21" s="17" t="inlineStr">
         <is>
@@ -2346,6 +2574,7 @@
         </is>
       </c>
     </row>
+    <row r="27"/>
     <row r="28">
       <c r="A28" s="21" t="inlineStr">
         <is>
@@ -2353,6 +2582,7 @@
         </is>
       </c>
     </row>
+    <row r="29"/>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
@@ -2530,6 +2760,7 @@
       <c r="B50" s="2" t="inlineStr"/>
       <c r="C50" s="2" t="inlineStr"/>
     </row>
+    <row r="51"/>
     <row r="52">
       <c r="A52" s="9" t="inlineStr">
         <is>
@@ -2537,6 +2768,7 @@
         </is>
       </c>
     </row>
+    <row r="53"/>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
@@ -2551,6 +2783,7 @@
         </is>
       </c>
     </row>
+    <row r="56"/>
     <row r="57">
       <c r="A57" s="19" t="inlineStr">
         <is>
@@ -2565,6 +2798,7 @@
         </is>
       </c>
     </row>
+    <row r="59"/>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
@@ -2593,6 +2827,7 @@
         </is>
       </c>
     </row>
+    <row r="64"/>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
@@ -2614,6 +2849,7 @@
         </is>
       </c>
     </row>
+    <row r="68"/>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
@@ -2628,6 +2864,7 @@
         </is>
       </c>
     </row>
+    <row r="71"/>
     <row r="72">
       <c r="A72" s="20" t="inlineStr">
         <is>
@@ -2642,6 +2879,7 @@
         </is>
       </c>
     </row>
+    <row r="74"/>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
@@ -2684,6 +2922,7 @@
         </is>
       </c>
     </row>
+    <row r="81"/>
     <row r="82">
       <c r="A82" s="21" t="inlineStr">
         <is>
@@ -2691,6 +2930,7 @@
         </is>
       </c>
     </row>
+    <row r="83"/>
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
@@ -3100,6 +3340,7 @@
       <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="2" t="inlineStr"/>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -4249,6 +4490,7 @@
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="2" t="inlineStr"/>
     </row>
+    <row r="12"/>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
@@ -5306,7 +5548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5411,6 +5653,7 @@
       <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="2" t="inlineStr"/>
     </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" s="21" t="inlineStr">
         <is>
@@ -5418,6 +5661,7 @@
         </is>
       </c>
     </row>
+    <row r="15"/>
     <row r="16">
       <c r="A16" s="23" t="inlineStr">
         <is>
@@ -5446,6 +5690,7 @@
         </is>
       </c>
     </row>
+    <row r="20"/>
     <row r="21">
       <c r="A21" s="24" t="inlineStr">
         <is>
@@ -5481,6 +5726,7 @@
         </is>
       </c>
     </row>
+    <row r="26"/>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
@@ -5554,6 +5800,7 @@
       <c r="B35" s="2" t="inlineStr"/>
       <c r="C35" s="2" t="inlineStr"/>
     </row>
+    <row r="36"/>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
@@ -6560,6 +6807,8 @@
       <c r="B160" s="2" t="inlineStr"/>
       <c r="C160" s="2" t="inlineStr"/>
     </row>
+    <row r="161"/>
+    <row r="162"/>
     <row r="163">
       <c r="A163" s="25" t="inlineStr">
         <is>
@@ -6567,6 +6816,7 @@
         </is>
       </c>
     </row>
+    <row r="164"/>
     <row r="165">
       <c r="A165" s="9" t="inlineStr">
         <is>
@@ -6588,6 +6838,7 @@
         </is>
       </c>
     </row>
+    <row r="168"/>
     <row r="169">
       <c r="A169" s="26" t="inlineStr">
         <is>
@@ -6595,6 +6846,8 @@
         </is>
       </c>
     </row>
+    <row r="170"/>
+    <row r="171"/>
     <row r="172">
       <c r="A172" s="25" t="inlineStr">
         <is>
@@ -6602,6 +6855,7 @@
         </is>
       </c>
     </row>
+    <row r="173"/>
     <row r="174">
       <c r="A174" s="9" t="inlineStr">
         <is>
@@ -6623,6 +6877,7 @@
         </is>
       </c>
     </row>
+    <row r="177"/>
     <row r="178">
       <c r="A178" s="26" t="inlineStr">
         <is>
@@ -6630,6 +6885,8 @@
         </is>
       </c>
     </row>
+    <row r="179"/>
+    <row r="180"/>
     <row r="181">
       <c r="A181" s="25" t="inlineStr">
         <is>
@@ -6637,6 +6894,7 @@
         </is>
       </c>
     </row>
+    <row r="182"/>
     <row r="183">
       <c r="A183" s="9" t="inlineStr">
         <is>
@@ -6658,6 +6916,7 @@
         </is>
       </c>
     </row>
+    <row r="186"/>
     <row r="187">
       <c r="A187" s="26" t="inlineStr">
         <is>
@@ -6665,6 +6924,8 @@
         </is>
       </c>
     </row>
+    <row r="188"/>
+    <row r="189"/>
     <row r="190">
       <c r="A190" s="25" t="inlineStr">
         <is>
@@ -6672,6 +6933,7 @@
         </is>
       </c>
     </row>
+    <row r="191"/>
     <row r="192">
       <c r="A192" s="9" t="inlineStr">
         <is>
@@ -6693,6 +6955,7 @@
         </is>
       </c>
     </row>
+    <row r="195"/>
     <row r="196">
       <c r="A196" s="26" t="inlineStr">
         <is>
@@ -6700,6 +6963,8 @@
         </is>
       </c>
     </row>
+    <row r="197"/>
+    <row r="198"/>
     <row r="199">
       <c r="A199" s="25" t="inlineStr">
         <is>
@@ -6707,6 +6972,7 @@
         </is>
       </c>
     </row>
+    <row r="200"/>
     <row r="201">
       <c r="A201" s="9" t="inlineStr">
         <is>
@@ -6728,6 +6994,7 @@
         </is>
       </c>
     </row>
+    <row r="204"/>
     <row r="205">
       <c r="A205" s="26" t="inlineStr">
         <is>
@@ -6735,6 +7002,8 @@
         </is>
       </c>
     </row>
+    <row r="206"/>
+    <row r="207"/>
     <row r="208">
       <c r="A208" s="25" t="inlineStr">
         <is>
@@ -6742,6 +7011,7 @@
         </is>
       </c>
     </row>
+    <row r="209"/>
     <row r="210">
       <c r="A210" s="9" t="inlineStr">
         <is>
@@ -6763,8 +7033,48 @@
         </is>
       </c>
     </row>
+    <row r="213"/>
     <row r="214">
       <c r="A214" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217">
+      <c r="A217" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="218"/>
+    <row r="219">
+      <c r="A219" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="222"/>
+    <row r="223">
+      <c r="A223" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>
@@ -6803,6 +7113,7 @@
       <c r="B1" s="2" t="inlineStr"/>
       <c r="C1" s="2" t="inlineStr"/>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -7732,6 +8043,7 @@
         </is>
       </c>
     </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" s="21" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update Excel guides to v11202116
VERSION: 11202116 (Nov 20, 21:21 KST)

UPDATES:
- Version header updated in both EN and KR guides
- Previous version content preserved
- Column widths optimized for readability

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_EN.xlsx
+++ b/docs/VRS_Manager_Process_Guide_EN.xlsx
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C276"/>
+  <dimension ref="A1:C311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Version 1121.0 (Phase 3.1.1 - Word-Level Diff Enhancement)</t>
+          <t>Version 11202116 (DateTime Versioning Build)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -2359,6 +2359,233 @@
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
+        </is>
+      </c>
+    </row>
+    <row r="277"/>
+    <row r="278"/>
+    <row r="279">
+      <c r="A279" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v1.121.0?</t>
+        </is>
+      </c>
+    </row>
+    <row r="280"/>
+    <row r="281">
+      <c r="A281" s="9" t="inlineStr">
+        <is>
+          <t>✅ Phase 3.1.1 COMPLETED - Word-Level Diff Enhancement (v1.121.0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IMPROVED: Word-level diff (cleaner output than character-level)</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: Separate 'Diff Detail' column showing exact changes [old→new]</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: Progress bar with filling animation during analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • NEW: StrOrigin Analysis now in BOTH Raw and Working Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IMPROVED: 4-column layout for better readability</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • ANALYSIS: Shows which StrOrigin changes are trivial vs substantial</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="9" t="inlineStr">
+        <is>
+          <t>✅ Critical Bug Fixes (v1118.6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: TypeError 'unhashable type: dict' in Working VRS Check</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: All DataFrame column access now uses safe_str() pattern</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • FIXED: Lookup dictionaries now correctly store indices (not dict objects)</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: 100% accuracy verified with 5000-row comprehensive test suite</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TESTED: All processors (Raw, Working, All Language) passing with real data</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="9" t="inlineStr">
+        <is>
+          <t>✅ Phase 2.2.1 COMPLETED - Super Group Analysis Improvements (v1118.4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REMOVED: 'Others' super group and stageclosedialog check entirely</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REORDERED: Super groups - AI Dialog now appears before Quest Dialog</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • RENAMED: 'Untranslated Words (Remaining to Translate)' → 'Not Translated'</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • REMOVED: Migration columns from main table (Words Migrated In/Out)</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • ADDED: Detailed 'Super Group Migrations' table below main table</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows source → destination pairs with word counts for all migrations</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • UPDATED: Explanatory notes below table (removed 'Others' references)</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 8 super groups total: Main Chapters, F1, F2, F3, AI Dialog, Quest Dialog, Other, Everything Else</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="9" t="inlineStr">
+        <is>
+          <t>Column Order (Reorganized for Better Readability):</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 1. Super Group Name, Total Words (Current/Previous), Net Change, % Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 2. Translated/Untranslated words, Translation % (Current/Previous/Change)</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • 3. Detailed breakdown: Words Added/Deleted/Changed/Unchanged/Migrated</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="9" t="inlineStr">
+        <is>
+          <t>✅ v1118.3 - Master File Update - TimeFrame Preservation Restored</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • TimeFrame = StartFrame ONLY (EndFrame always updates from SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed AND StrOrigin changed → Update StartFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • IF StartFrame changed BUT StrOrigin NOT changed → Preserve StartFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
         </is>
@@ -5548,7 +5775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7075,6 +7302,45 @@
     <row r="222"/>
     <row r="223">
       <c r="A223" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226">
+      <c r="A226" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="227"/>
+    <row r="228">
+      <c r="A228" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="231"/>
+    <row r="232">
+      <c r="A232" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>

<commit_message>
Update all documentation for Phase 4 features (v12031417)
CHANGES:
- Updated README.md/README_KR.md with Smart Change Classification section
- Added Output Columns documentation (CHANGES, DETAILED_CHANGES, PreviousEventName, PreviousText)
- Updated WIKI_CONFLUENCE.md with complete feature explanations
- Updated CHANGE_TYPES_REFERENCE.md with Priority Ranking System
- Regenerated Excel guides (EN/KR) with user-friendly feature presentation
- All docs now consistently reference v12031417

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_EN.xlsx
+++ b/docs/VRS_Manager_Process_Guide_EN.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="1. Raw Process" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2. Working Process" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="3. All Language" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="4. Master Update" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Workflow Guide" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Technical Reference" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Overview" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1. Raw Process" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2. Working Process" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3. All Language" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4. Master Update" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Workflow Guide" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Technical Reference" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C311"/>
+  <dimension ref="A1:C339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Version 11202116 (DateTime Versioning Build)</t>
+          <t>Version 12031417 (Smarter Change Detection + Enhanced Tracking)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -2588,6 +2588,184 @@
       <c r="A311" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Prevents unwanted timing updates when dialogue content unchanged</t>
+        </is>
+      </c>
+    </row>
+    <row r="312"/>
+    <row r="313"/>
+    <row r="314">
+      <c r="A314" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v12031417?</t>
+        </is>
+      </c>
+    </row>
+    <row r="315"/>
+    <row r="316">
+      <c r="A316" s="9" t="inlineStr">
+        <is>
+          <t>🎯 Smarter Change Classification</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES column now shows the MOST IMPORTANT change when multiple fields change</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Priority order: StrOrigin → Desc → CastingKey → TimeFrame → Group → EventName → SequenceName → DialogType → CharacterGroup</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: If EventName AND StrOrigin both changed → Shows 'StrOrigin Change' (higher priority)</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Makes it easier to quickly identify what needs attention first</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="9" t="inlineStr">
+        <is>
+          <t>📋 New DETAILED_CHANGES Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the FULL list of all changes when multiple fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: 'EventName+StrOrigin+Desc Change' - all 3 fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Located at the far right of the output for detailed review</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES = quick view, DETAILED_CHANGES = complete picture</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="9" t="inlineStr">
+        <is>
+          <t>🔄 New PreviousEventName Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • When EventName changes, you can now see what the OLD EventName was</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helps track row reorganization and event renaming</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Only populated when EventName actually changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty for New Rows and No Change rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="9" t="inlineStr">
+        <is>
+          <t>📝 New PreviousText Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the previous Text/Translation for ALL matched rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Instantly see what the old translation was without searching</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helpful for reviewing what needs re-translation</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty only for New Rows (no previous data exists)</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="9" t="inlineStr">
+        <is>
+          <t>🔧 Improved CastingKey Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CastingKey comparison is now more reliable across files</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Consistent handling even when files have different column structures</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
         </is>
       </c>
     </row>
@@ -3697,7 +3875,7 @@
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr"/>
@@ -3774,7 +3952,7 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr"/>
@@ -3879,7 +4057,7 @@
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr"/>
@@ -3956,7 +4134,7 @@
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr"/>
@@ -4033,7 +4211,7 @@
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr"/>
@@ -4119,7 +4297,7 @@
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr"/>
@@ -4196,7 +4374,7 @@
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr"/>
@@ -4255,7 +4433,7 @@
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr"/>
@@ -4810,7 +4988,7 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr"/>
@@ -5270,7 +5448,7 @@
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr"/>
@@ -5324,7 +5502,7 @@
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr"/>
@@ -5775,7 +5953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5998,7 +6176,7 @@
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr"/>
@@ -6129,7 +6307,7 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr"/>
@@ -6188,7 +6366,7 @@
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr"/>
@@ -6229,7 +6407,7 @@
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr"/>
@@ -6265,7 +6443,7 @@
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr"/>
@@ -6301,7 +6479,7 @@
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr"/>
@@ -6328,7 +6506,7 @@
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>  </t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr"/>
@@ -7341,6 +7519,45 @@
     <row r="231"/>
     <row r="232">
       <c r="A232" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235">
+      <c r="A235" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="236"/>
+    <row r="237">
+      <c r="A237" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="240"/>
+    <row r="241">
+      <c r="A241" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>

<commit_message>
v12051800: Settings toggle, Super Group improvements
- Add SETTINGS button with Priority Change toggle (ON/OFF)
- Add NarrationDialog to Super Group Word Analysis
- Add "Item" to Other super group cluster
- Main Chapters: keyword-based (chapter/intro/prolog/epilog)
- Add NET CHANGE explanation below analysis table
- Update all guides and documentation

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_EN.xlsx
+++ b/docs/VRS_Manager_Process_Guide_EN.xlsx
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C339"/>
+  <dimension ref="A1:C367"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Version 12031417 (Smarter Change Detection + Enhanced Tracking)</t>
+          <t>Version 12051800 (Smarter Change Detection + Enhanced Tracking)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -2764,6 +2764,184 @@
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
+        </is>
+      </c>
+    </row>
+    <row r="340"/>
+    <row r="341"/>
+    <row r="342">
+      <c r="A342" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v12051800?</t>
+        </is>
+      </c>
+    </row>
+    <row r="343"/>
+    <row r="344">
+      <c r="A344" s="9" t="inlineStr">
+        <is>
+          <t>🎯 Smarter Change Classification</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES column now shows the MOST IMPORTANT change when multiple fields change</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Priority order: StrOrigin → Desc → CastingKey → TimeFrame → Group → EventName → SequenceName → DialogType → CharacterGroup</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: If EventName AND StrOrigin both changed → Shows 'StrOrigin Change' (higher priority)</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Makes it easier to quickly identify what needs attention first</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="9" t="inlineStr">
+        <is>
+          <t>📋 New DETAILED_CHANGES Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the FULL list of all changes when multiple fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: 'EventName+StrOrigin+Desc Change' - all 3 fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Located at the far right of the output for detailed review</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES = quick view, DETAILED_CHANGES = complete picture</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="9" t="inlineStr">
+        <is>
+          <t>🔄 New PreviousEventName Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • When EventName changes, you can now see what the OLD EventName was</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helps track row reorganization and event renaming</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Only populated when EventName actually changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty for New Rows and No Change rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="9" t="inlineStr">
+        <is>
+          <t>📝 New PreviousText Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the previous Text/Translation for ALL matched rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Instantly see what the old translation was without searching</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helpful for reviewing what needs re-translation</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty only for New Rows (no previous data exists)</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="9" t="inlineStr">
+        <is>
+          <t>🔧 Improved CastingKey Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CastingKey comparison is now more reliable across files</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Consistent handling even when files have different column structures</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
         </is>
@@ -5953,7 +6131,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C241"/>
+  <dimension ref="A1:C250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7558,6 +7736,45 @@
     <row r="240"/>
     <row r="241">
       <c r="A241" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244">
+      <c r="A244" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="245"/>
+    <row r="246">
+      <c r="A246" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="249"/>
+    <row r="250">
+      <c r="A250" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>

<commit_message>
v12051333: Add timestamp validation safety check
- Add timestamp validation to check_version_unified.py
- Version must be within 1 hour of current time (MMDDHHMM format)
- Build blocked if version timestamp too far from now
- Fixes incorrect version 12051800 → 12051333

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_EN.xlsx
+++ b/docs/VRS_Manager_Process_Guide_EN.xlsx
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C367"/>
+  <dimension ref="A1:C395"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Version 12051800 (Smarter Change Detection + Enhanced Tracking)</t>
+          <t>Version 12051333 (Smarter Change Detection + Enhanced Tracking)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -2942,6 +2942,184 @@
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
+        </is>
+      </c>
+    </row>
+    <row r="368"/>
+    <row r="369"/>
+    <row r="370">
+      <c r="A370" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v12051333?</t>
+        </is>
+      </c>
+    </row>
+    <row r="371"/>
+    <row r="372">
+      <c r="A372" s="9" t="inlineStr">
+        <is>
+          <t>🎯 Smarter Change Classification</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES column now shows the MOST IMPORTANT change when multiple fields change</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Priority order: StrOrigin → Desc → CastingKey → TimeFrame → Group → EventName → SequenceName → DialogType → CharacterGroup</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: If EventName AND StrOrigin both changed → Shows 'StrOrigin Change' (higher priority)</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Makes it easier to quickly identify what needs attention first</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="9" t="inlineStr">
+        <is>
+          <t>📋 New DETAILED_CHANGES Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the FULL list of all changes when multiple fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: 'EventName+StrOrigin+Desc Change' - all 3 fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Located at the far right of the output for detailed review</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES = quick view, DETAILED_CHANGES = complete picture</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="9" t="inlineStr">
+        <is>
+          <t>🔄 New PreviousEventName Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • When EventName changes, you can now see what the OLD EventName was</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helps track row reorganization and event renaming</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Only populated when EventName actually changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty for New Rows and No Change rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="9" t="inlineStr">
+        <is>
+          <t>📝 New PreviousText Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the previous Text/Translation for ALL matched rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Instantly see what the old translation was without searching</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helpful for reviewing what needs re-translation</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty only for New Rows (no previous data exists)</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="9" t="inlineStr">
+        <is>
+          <t>🔧 Improved CastingKey Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CastingKey comparison is now more reliable across files</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Consistent handling even when files have different column structures</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
         </is>
@@ -6131,7 +6309,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C250"/>
+  <dimension ref="A1:C259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7775,6 +7953,45 @@
     <row r="249"/>
     <row r="250">
       <c r="A250" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="251"/>
+    <row r="252"/>
+    <row r="253">
+      <c r="A253" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="254"/>
+    <row r="255">
+      <c r="A255" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="258"/>
+    <row r="259">
+      <c r="A259" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>

<commit_message>
v12051348: Super Group order fix, Narration Dialog naming
- Fix super group table order: Main Chapters, Faction 1-3, AI Dialog, Quest Dialog, Narration Dialog, Other, Everything Else
- Rename NarrationDialog → Narration Dialog (with space)
- Remove sorted() - use custom order for display
- Migration tracking uses same super group set

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/VRS_Manager_Process_Guide_EN.xlsx
+++ b/docs/VRS_Manager_Process_Guide_EN.xlsx
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C395"/>
+  <dimension ref="A1:C423"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Version 12051333 (Smarter Change Detection + Enhanced Tracking)</t>
+          <t>Version 12051348 (Smarter Change Detection + Enhanced Tracking)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr"/>
@@ -3120,6 +3120,184 @@
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
+        </is>
+      </c>
+    </row>
+    <row r="396"/>
+    <row r="397"/>
+    <row r="398">
+      <c r="A398" s="8" t="inlineStr">
+        <is>
+          <t>WHAT'S NEW IN v12051348?</t>
+        </is>
+      </c>
+    </row>
+    <row r="399"/>
+    <row r="400">
+      <c r="A400" s="9" t="inlineStr">
+        <is>
+          <t>🎯 Smarter Change Classification</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES column now shows the MOST IMPORTANT change when multiple fields change</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Priority order: StrOrigin → Desc → CastingKey → TimeFrame → Group → EventName → SequenceName → DialogType → CharacterGroup</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: If EventName AND StrOrigin both changed → Shows 'StrOrigin Change' (higher priority)</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Makes it easier to quickly identify what needs attention first</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="9" t="inlineStr">
+        <is>
+          <t>📋 New DETAILED_CHANGES Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the FULL list of all changes when multiple fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Example: 'EventName+StrOrigin+Desc Change' - all 3 fields changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Located at the far right of the output for detailed review</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CHANGES = quick view, DETAILED_CHANGES = complete picture</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="9" t="inlineStr">
+        <is>
+          <t>🔄 New PreviousEventName Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • When EventName changes, you can now see what the OLD EventName was</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helps track row reorganization and event renaming</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Only populated when EventName actually changed</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty for New Rows and No Change rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="9" t="inlineStr">
+        <is>
+          <t>📝 New PreviousText Column</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Shows the previous Text/Translation for ALL matched rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Instantly see what the old translation was without searching</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Helpful for reviewing what needs re-translation</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Empty only for New Rows (no previous data exists)</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="9" t="inlineStr">
+        <is>
+          <t>🔧 Improved CastingKey Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • CastingKey comparison is now more reliable across files</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • Consistent handling even when files have different column structures</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
         <is>
           <t xml:space="preserve">  • Warnings displayed when source data is incomplete</t>
         </is>
@@ -6309,7 +6487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C259"/>
+  <dimension ref="A1:C268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7992,6 +8170,45 @@
     <row r="258"/>
     <row r="259">
       <c r="A259" s="26" t="inlineStr">
+        <is>
+          <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="260"/>
+    <row r="261"/>
+    <row r="262">
+      <c r="A262" s="25" t="inlineStr">
+        <is>
+          <t>TimeFrame Preservation Logic (v1117 - High Importance Only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="263"/>
+    <row r="264">
+      <c r="A264" s="9" t="inlineStr">
+        <is>
+          <t>Rule:</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed AND StrOrigin changed → Update TimeFrame (use SOURCE)</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  • If TimeFrame changed BUT StrOrigin did NOT change → Preserve TimeFrame (keep TARGET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="267"/>
+    <row r="268">
+      <c r="A268" s="26" t="inlineStr">
         <is>
           <t>This ensures TimeFrame updates only apply when accompanied by dialogue content changes.</t>
         </is>

</xml_diff>